<commit_message>
Revision to the dataset, R markdown and checklist.
In the dataset: I revised a few numbers as there was a new poster for the two phase III trials. There are no exact SDs, and information about dropouts. Thus, the risk of bias can be better evalauted and now have low risk of bias. Need to double-check the data with Oxford RAs.

In the Rmarkdwon: After follow-up with Virginia, I did not use HK corrections (<5 studies), but this can be changed back if needed. I also re-run the markdown using the updated dataset and updated the SoE tables. Potential refinemenets are needed.

In the checklist: I reported that HK corrections were not done, as <5 studies. I also reported that sensitivity analyses cannot be done as not studies to be excluded (e.g., no studies used imputed values, and no studies had not a low risk of bias).
</commit_message>
<xml_diff>
--- a/data/LSR3_H_2023-11-24.xlsx
+++ b/data/LSR3_H_2023-11-24.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/LRZ Sync+Share/Projects/GALENOS/3. systematic reviews/taar/4_analysis/lsr3_rmarkdown/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/Documents/GitHub/LSR3_taar1_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000ACE7-8810-264A-A282-D65E07339DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE108DC6-F301-D645-9602-F2D319FBA648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21880" yWindow="-18280" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="245">
   <si>
     <t>arm_name</t>
   </si>
@@ -472,9 +472,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Isaacson (2023)</t>
   </si>
   <si>
@@ -544,9 +541,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>Koblan (2020)</t>
   </si>
   <si>
@@ -595,18 +589,12 @@
     <t>&gt;18</t>
   </si>
   <si>
-    <t>145</t>
-  </si>
-  <si>
     <t>ulotaront 75mg/d (adults)</t>
   </si>
   <si>
     <t>75</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
     <t>placebo (adults)</t>
   </si>
   <si>
@@ -619,19 +607,10 @@
     <t>464</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
     <t>ulotaront 100mg/d</t>
   </si>
   <si>
     <t>100</t>
-  </si>
-  <si>
-    <t>31</t>
   </si>
   <si>
     <t>24</t>
@@ -811,12 +790,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -831,11 +822,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,14 +1137,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DY26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="34" max="34" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:129" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1546,34 +1542,34 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
         <v>129</v>
       </c>
       <c r="F2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" t="s">
         <v>149</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>150</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>151</v>
-      </c>
-      <c r="I2" t="s">
-        <v>152</v>
       </c>
       <c r="J2">
         <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L2">
         <v>4</v>
@@ -1582,19 +1578,19 @@
         <v>6</v>
       </c>
       <c r="N2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" t="s">
         <v>154</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>155</v>
-      </c>
-      <c r="R2" t="s">
-        <v>156</v>
       </c>
       <c r="S2" t="s">
         <v>144</v>
       </c>
       <c r="T2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U2" t="s">
         <v>144</v>
@@ -1606,31 +1602,31 @@
         <v>144</v>
       </c>
       <c r="X2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y2" t="s">
         <v>144</v>
       </c>
       <c r="Z2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB2" t="s">
         <v>159</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE2" t="s">
         <v>159</v>
       </c>
-      <c r="AB2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>160</v>
-      </c>
       <c r="AF2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG2">
         <v>23</v>
@@ -1651,7 +1647,7 @@
         <v>135</v>
       </c>
       <c r="AN2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AO2">
         <v>24</v>
@@ -1675,7 +1671,7 @@
         <v>135</v>
       </c>
       <c r="BL2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BM2">
         <v>23</v>
@@ -1732,7 +1728,7 @@
         <v>141</v>
       </c>
       <c r="DX2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY2" t="s">
         <v>135</v>
@@ -1740,37 +1736,37 @@
     </row>
     <row r="3" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
         <v>131</v>
       </c>
       <c r="G3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" t="s">
         <v>150</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>151</v>
-      </c>
-      <c r="I3" t="s">
-        <v>152</v>
       </c>
       <c r="J3">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1779,55 +1775,55 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O3" t="s">
         <v>145</v>
       </c>
       <c r="R3" t="s">
+        <v>166</v>
+      </c>
+      <c r="S3" t="s">
         <v>167</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>168</v>
       </c>
-      <c r="T3" t="s">
-        <v>169</v>
-      </c>
       <c r="U3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V3" t="s">
         <v>131</v>
       </c>
       <c r="W3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X3" t="s">
         <v>131</v>
       </c>
       <c r="Y3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB3" t="s">
         <v>159</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE3" t="s">
         <v>159</v>
       </c>
-      <c r="AB3" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>160</v>
-      </c>
       <c r="AF3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG3">
         <v>14</v>
@@ -1848,7 +1844,7 @@
         <v>135</v>
       </c>
       <c r="AN3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AO3">
         <v>14</v>
@@ -1872,7 +1868,7 @@
         <v>135</v>
       </c>
       <c r="BL3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BM3">
         <v>14</v>
@@ -1944,10 +1940,10 @@
         <v>14</v>
       </c>
       <c r="DW3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY3" t="s">
         <v>135</v>
@@ -1958,34 +1954,34 @@
         <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
         <v>129</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G4" t="s">
         <v>130</v>
       </c>
       <c r="H4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J4">
         <v>120</v>
       </c>
       <c r="K4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L4">
         <v>43</v>
@@ -1997,49 +1993,49 @@
         <v>142</v>
       </c>
       <c r="O4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="T4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="V4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="X4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Z4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF4" t="s">
         <v>132</v>
@@ -2162,7 +2158,7 @@
         <v>135</v>
       </c>
       <c r="CJ4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CK4" t="s">
         <v>140</v>
@@ -2255,7 +2251,7 @@
         <v>141</v>
       </c>
       <c r="DX4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY4" t="s">
         <v>135</v>
@@ -2263,19 +2259,19 @@
     </row>
     <row r="5" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" t="s">
         <v>131</v>
@@ -2284,16 +2280,16 @@
         <v>130</v>
       </c>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J5">
         <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L5">
         <v>46</v>
@@ -2302,52 +2298,52 @@
         <v>4</v>
       </c>
       <c r="N5" t="s">
+        <v>176</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="R5" t="s">
+        <v>174</v>
+      </c>
+      <c r="S5" t="s">
+        <v>177</v>
+      </c>
+      <c r="T5" t="s">
         <v>178</v>
       </c>
-      <c r="O5" t="s">
-        <v>179</v>
-      </c>
-      <c r="R5" t="s">
-        <v>176</v>
-      </c>
-      <c r="S5" t="s">
-        <v>179</v>
-      </c>
-      <c r="T5" t="s">
-        <v>180</v>
-      </c>
       <c r="U5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="V5" t="s">
         <v>131</v>
       </c>
       <c r="W5" t="s">
+        <v>177</v>
+      </c>
+      <c r="X5" t="s">
         <v>179</v>
       </c>
-      <c r="X5" t="s">
-        <v>181</v>
-      </c>
       <c r="Y5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Z5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD5" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF5" t="s">
         <v>132</v>
@@ -2470,7 +2466,7 @@
         <v>135</v>
       </c>
       <c r="CJ5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CK5" t="s">
         <v>140</v>
@@ -2560,10 +2556,10 @@
         <v>125</v>
       </c>
       <c r="DW5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY5" t="s">
         <v>135</v>
@@ -2571,76 +2567,85 @@
     </row>
     <row r="6" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
         <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G6" t="s">
         <v>130</v>
       </c>
       <c r="H6" t="s">
-        <v>151</v>
-      </c>
-      <c r="I6" t="s">
-        <v>185</v>
-      </c>
-      <c r="J6">
-        <v>145</v>
+        <v>150</v>
+      </c>
+      <c r="I6" s="2">
+        <v>435</v>
+      </c>
+      <c r="J6" s="3">
+        <v>144</v>
       </c>
       <c r="K6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M6">
         <v>6</v>
       </c>
-      <c r="N6" t="s">
-        <v>146</v>
-      </c>
-      <c r="O6" t="s">
-        <v>187</v>
+      <c r="N6" s="2">
+        <v>22</v>
+      </c>
+      <c r="O6" s="3">
+        <v>144</v>
+      </c>
+      <c r="R6" s="2">
+        <v>34</v>
+      </c>
+      <c r="S6" s="2">
+        <v>144</v>
       </c>
       <c r="Z6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB6" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF6" t="s">
         <v>132</v>
       </c>
-      <c r="AG6">
-        <v>145</v>
+      <c r="AG6" s="2">
+        <v>142</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>102</v>
       </c>
       <c r="AI6">
         <v>-16.899999999999999</v>
       </c>
-      <c r="AJ6">
-        <v>20</v>
+      <c r="AJ6" s="2">
+        <v>19.07</v>
       </c>
       <c r="AK6" t="s">
         <v>133</v>
@@ -2649,13 +2654,13 @@
         <v>134</v>
       </c>
       <c r="AM6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW6" t="s">
         <v>141</v>
       </c>
       <c r="DX6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY6" t="s">
         <v>135</v>
@@ -2663,76 +2668,85 @@
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G7" t="s">
         <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J7">
+        <v>150</v>
+      </c>
+      <c r="I7" s="2">
+        <v>435</v>
+      </c>
+      <c r="J7" s="3">
         <v>145</v>
       </c>
       <c r="K7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
-      <c r="N7" t="s">
-        <v>190</v>
-      </c>
-      <c r="O7" t="s">
-        <v>187</v>
+      <c r="N7" s="2">
+        <v>29</v>
+      </c>
+      <c r="O7" s="3">
+        <v>145</v>
+      </c>
+      <c r="R7" s="2">
+        <v>27</v>
+      </c>
+      <c r="S7" s="2">
+        <v>145</v>
       </c>
       <c r="Z7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA7" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB7" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC7" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF7" t="s">
         <v>132</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="2">
         <v>145</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>102</v>
       </c>
       <c r="AI7">
         <v>-19.600000000000001</v>
       </c>
-      <c r="AJ7">
-        <v>20</v>
+      <c r="AJ7" s="2">
+        <v>19.27</v>
       </c>
       <c r="AK7" t="s">
         <v>133</v>
@@ -2741,13 +2755,13 @@
         <v>134</v>
       </c>
       <c r="AM7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW7" t="s">
         <v>141</v>
       </c>
       <c r="DX7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY7" t="s">
         <v>135</v>
@@ -2755,19 +2769,19 @@
     </row>
     <row r="8" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F8" t="s">
         <v>131</v>
@@ -2776,43 +2790,49 @@
         <v>130</v>
       </c>
       <c r="H8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J8">
-        <v>145</v>
+        <v>183</v>
+      </c>
+      <c r="J8" s="3">
+        <v>146</v>
       </c>
       <c r="K8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M8">
         <v>6</v>
       </c>
-      <c r="N8" t="s">
-        <v>170</v>
-      </c>
-      <c r="O8" t="s">
-        <v>187</v>
+      <c r="N8" s="2">
+        <v>26</v>
+      </c>
+      <c r="O8" s="3">
+        <v>146</v>
+      </c>
+      <c r="R8" s="2">
+        <v>27</v>
+      </c>
+      <c r="S8" s="2">
+        <v>146</v>
       </c>
       <c r="Z8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB8" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF8" t="s">
         <v>132</v>
@@ -2820,11 +2840,14 @@
       <c r="AG8">
         <v>145</v>
       </c>
+      <c r="AH8" s="2">
+        <v>102</v>
+      </c>
       <c r="AI8">
         <v>-19.3</v>
       </c>
-      <c r="AJ8">
-        <v>20</v>
+      <c r="AJ8" s="2">
+        <v>18.059999999999999</v>
       </c>
       <c r="AK8" t="s">
         <v>133</v>
@@ -2833,13 +2856,13 @@
         <v>134</v>
       </c>
       <c r="AM8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY8" t="s">
         <v>135</v>
@@ -2847,76 +2870,85 @@
     </row>
     <row r="9" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
         <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G9" t="s">
         <v>130</v>
       </c>
       <c r="H9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I9" t="s">
-        <v>194</v>
-      </c>
-      <c r="J9">
-        <v>154</v>
+        <v>190</v>
+      </c>
+      <c r="J9" s="2">
+        <v>155</v>
       </c>
       <c r="K9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M9">
         <v>6</v>
       </c>
-      <c r="N9" t="s">
-        <v>195</v>
-      </c>
-      <c r="O9" t="s">
-        <v>196</v>
+      <c r="N9" s="2">
+        <v>23</v>
+      </c>
+      <c r="O9" s="2">
+        <v>155</v>
+      </c>
+      <c r="R9" s="2">
+        <v>34</v>
+      </c>
+      <c r="S9" s="2">
+        <v>155</v>
       </c>
       <c r="Z9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB9" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB9" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF9" t="s">
         <v>132</v>
       </c>
-      <c r="AG9">
-        <v>154</v>
+      <c r="AG9" s="2">
+        <v>153</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>101</v>
       </c>
       <c r="AI9">
         <v>-16.399999999999999</v>
       </c>
-      <c r="AJ9">
-        <v>20</v>
+      <c r="AJ9" s="2">
+        <v>18.55</v>
       </c>
       <c r="AK9" t="s">
         <v>133</v>
@@ -2925,13 +2957,13 @@
         <v>134</v>
       </c>
       <c r="AM9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW9" t="s">
         <v>141</v>
       </c>
       <c r="DX9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY9" t="s">
         <v>135</v>
@@ -2939,76 +2971,85 @@
     </row>
     <row r="10" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
         <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G10" t="s">
         <v>130</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>194</v>
-      </c>
-      <c r="J10">
+        <v>190</v>
+      </c>
+      <c r="J10" s="2">
         <v>154</v>
       </c>
       <c r="K10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M10">
         <v>6</v>
       </c>
-      <c r="N10" t="s">
-        <v>199</v>
-      </c>
-      <c r="O10" t="s">
-        <v>196</v>
+      <c r="N10" s="2">
+        <v>27</v>
+      </c>
+      <c r="O10" s="2">
+        <v>154</v>
+      </c>
+      <c r="R10" s="2">
+        <v>38</v>
+      </c>
+      <c r="S10" s="2">
+        <v>154</v>
       </c>
       <c r="Z10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA10" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB10" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB10" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC10" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF10" t="s">
         <v>132</v>
       </c>
-      <c r="AG10">
-        <v>154</v>
+      <c r="AG10" s="2">
+        <v>152</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>100</v>
       </c>
       <c r="AI10">
         <v>-18.100000000000001</v>
       </c>
-      <c r="AJ10">
-        <v>20</v>
+      <c r="AJ10" s="2">
+        <v>18.489999999999998</v>
       </c>
       <c r="AK10" t="s">
         <v>133</v>
@@ -3017,13 +3058,13 @@
         <v>134</v>
       </c>
       <c r="AM10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW10" t="s">
         <v>141</v>
       </c>
       <c r="DX10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY10" t="s">
         <v>135</v>
@@ -3031,19 +3072,19 @@
     </row>
     <row r="11" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" t="s">
         <v>131</v>
@@ -3052,55 +3093,64 @@
         <v>130</v>
       </c>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I11" t="s">
-        <v>194</v>
-      </c>
-      <c r="J11">
-        <v>154</v>
+        <v>190</v>
+      </c>
+      <c r="J11" s="2">
+        <v>155</v>
       </c>
       <c r="K11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M11">
         <v>6</v>
       </c>
-      <c r="N11" t="s">
-        <v>200</v>
-      </c>
-      <c r="O11" t="s">
-        <v>196</v>
+      <c r="N11" s="2">
+        <v>21</v>
+      </c>
+      <c r="O11" s="2">
+        <v>155</v>
+      </c>
+      <c r="R11" s="2">
+        <v>27</v>
+      </c>
+      <c r="S11" s="2">
+        <v>155</v>
       </c>
       <c r="Z11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA11" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB11" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB11" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC11" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF11" t="s">
         <v>132</v>
       </c>
-      <c r="AG11">
-        <v>154</v>
+      <c r="AG11" s="2">
+        <v>155</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>100</v>
       </c>
       <c r="AI11">
         <v>-14.3</v>
       </c>
-      <c r="AJ11">
-        <v>20</v>
+      <c r="AJ11" s="2">
+        <v>18.670000000000002</v>
       </c>
       <c r="AK11" t="s">
         <v>133</v>
@@ -3109,13 +3159,13 @@
         <v>134</v>
       </c>
       <c r="AM11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY11" t="s">
         <v>135</v>
@@ -3123,19 +3173,19 @@
     </row>
     <row r="12" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" t="s">
         <v>131</v>
@@ -3144,16 +3194,16 @@
         <v>130</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J12">
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L12">
         <v>19</v>
@@ -3162,52 +3212,52 @@
         <v>4</v>
       </c>
       <c r="N12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="R12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="S12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="T12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="V12" t="s">
         <v>131</v>
       </c>
       <c r="W12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="X12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="Z12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD12" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF12" t="s">
         <v>132</v>
@@ -3225,7 +3275,7 @@
         <v>20.18</v>
       </c>
       <c r="AK12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL12" t="s">
         <v>135</v>
@@ -3249,7 +3299,7 @@
         <v>6.64</v>
       </c>
       <c r="AS12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT12" t="s">
         <v>135</v>
@@ -3273,7 +3323,7 @@
         <v>5.81</v>
       </c>
       <c r="BA12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB12" t="s">
         <v>135</v>
@@ -3282,7 +3332,7 @@
         <v>135</v>
       </c>
       <c r="BT12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU12">
         <v>54</v>
@@ -3297,7 +3347,7 @@
         <v>4.03</v>
       </c>
       <c r="BY12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ12" t="s">
         <v>135</v>
@@ -3348,10 +3398,10 @@
         <v>72</v>
       </c>
       <c r="DW12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY12" t="s">
         <v>135</v>
@@ -3359,37 +3409,37 @@
     </row>
     <row r="13" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F13" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="G13" t="s">
         <v>130</v>
       </c>
       <c r="H13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I13" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J13">
         <v>71</v>
       </c>
       <c r="K13" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L13">
         <v>19</v>
@@ -3398,52 +3448,52 @@
         <v>4</v>
       </c>
       <c r="N13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O13" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="R13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S13" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="T13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U13" t="s">
-        <v>214</v>
-      </c>
-      <c r="V13" t="s">
-        <v>158</v>
+        <v>207</v>
+      </c>
+      <c r="V13" s="5">
+        <v>0</v>
       </c>
       <c r="W13" t="s">
-        <v>213</v>
-      </c>
-      <c r="X13" t="s">
-        <v>131</v>
+        <v>206</v>
+      </c>
+      <c r="X13" s="5">
+        <v>2</v>
       </c>
       <c r="Y13" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="Z13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD13" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF13" t="s">
         <v>132</v>
@@ -3461,7 +3511,7 @@
         <v>17.03</v>
       </c>
       <c r="AK13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL13" t="s">
         <v>135</v>
@@ -3485,7 +3535,7 @@
         <v>6.14</v>
       </c>
       <c r="AS13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT13" t="s">
         <v>135</v>
@@ -3509,7 +3559,7 @@
         <v>5.85</v>
       </c>
       <c r="BA13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB13" t="s">
         <v>135</v>
@@ -3518,7 +3568,7 @@
         <v>135</v>
       </c>
       <c r="BT13" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU13">
         <v>49</v>
@@ -3533,7 +3583,7 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="BY13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ13" t="s">
         <v>135</v>
@@ -3587,7 +3637,7 @@
         <v>141</v>
       </c>
       <c r="DX13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY13" t="s">
         <v>135</v>
@@ -3595,37 +3645,37 @@
     </row>
     <row r="14" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F14" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G14" t="s">
         <v>130</v>
       </c>
       <c r="H14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I14" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J14">
         <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L14">
         <v>15</v>
@@ -3634,52 +3684,52 @@
         <v>4</v>
       </c>
       <c r="N14" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" t="s">
+        <v>210</v>
+      </c>
+      <c r="R14" t="s">
         <v>154</v>
       </c>
-      <c r="O14" t="s">
-        <v>217</v>
-      </c>
-      <c r="R14" t="s">
-        <v>155</v>
-      </c>
       <c r="S14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="T14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="V14" t="s">
         <v>131</v>
       </c>
       <c r="W14" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="X14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y14" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="Z14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD14" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF14" t="s">
         <v>132</v>
@@ -3697,7 +3747,7 @@
         <v>17.670000000000002</v>
       </c>
       <c r="AK14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL14" t="s">
         <v>135</v>
@@ -3721,7 +3771,7 @@
         <v>6.5</v>
       </c>
       <c r="AS14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT14" t="s">
         <v>135</v>
@@ -3745,7 +3795,7 @@
         <v>5.41</v>
       </c>
       <c r="BA14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB14" t="s">
         <v>135</v>
@@ -3754,7 +3804,7 @@
         <v>135</v>
       </c>
       <c r="BT14" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU14">
         <v>51</v>
@@ -3769,7 +3819,7 @@
         <v>4.08</v>
       </c>
       <c r="BY14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ14" t="s">
         <v>135</v>
@@ -3823,7 +3873,7 @@
         <v>141</v>
       </c>
       <c r="DX14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY14" t="s">
         <v>135</v>
@@ -3831,37 +3881,37 @@
     </row>
     <row r="15" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G15" t="s">
         <v>130</v>
       </c>
       <c r="H15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I15" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J15">
         <v>74</v>
       </c>
       <c r="K15" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L15">
         <v>18</v>
@@ -3870,52 +3920,52 @@
         <v>4</v>
       </c>
       <c r="N15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O15" t="s">
+        <v>207</v>
+      </c>
+      <c r="R15" t="s">
+        <v>167</v>
+      </c>
+      <c r="S15" t="s">
         <v>214</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>168</v>
       </c>
-      <c r="S15" t="s">
-        <v>221</v>
-      </c>
-      <c r="T15" t="s">
-        <v>169</v>
-      </c>
       <c r="U15" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="V15" t="s">
         <v>131</v>
       </c>
       <c r="W15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="X15" t="s">
         <v>131</v>
       </c>
       <c r="Y15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="Z15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD15" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF15" t="s">
         <v>132</v>
@@ -3933,7 +3983,7 @@
         <v>15.78</v>
       </c>
       <c r="AK15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL15" t="s">
         <v>135</v>
@@ -3957,7 +4007,7 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="AS15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT15" t="s">
         <v>135</v>
@@ -3981,7 +4031,7 @@
         <v>5.13</v>
       </c>
       <c r="BA15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB15" t="s">
         <v>135</v>
@@ -3990,7 +4040,7 @@
         <v>135</v>
       </c>
       <c r="BT15" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU15">
         <v>56</v>
@@ -4005,7 +4055,7 @@
         <v>4.09</v>
       </c>
       <c r="BY15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ15" t="s">
         <v>135</v>
@@ -4056,10 +4106,10 @@
         <v>71</v>
       </c>
       <c r="DW15" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="DX15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY15" t="s">
         <v>135</v>
@@ -4067,34 +4117,34 @@
     </row>
     <row r="16" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B16" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F16" t="s">
         <v>131</v>
       </c>
       <c r="G16" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I16" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J16">
         <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="L16">
         <v>18</v>
@@ -4103,28 +4153,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="T16" t="s">
         <v>131</v>
       </c>
       <c r="U16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="V16" t="s">
         <v>131</v>
       </c>
       <c r="W16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="X16" t="s">
         <v>131</v>
       </c>
       <c r="Y16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="CS16">
         <v>16</v>
@@ -4169,10 +4219,10 @@
         <v>34</v>
       </c>
       <c r="DW16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX16" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY16" t="s">
         <v>135</v>
@@ -4180,34 +4230,34 @@
     </row>
     <row r="17" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
         <v>129</v>
       </c>
       <c r="F17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G17" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I17" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J17">
         <v>35</v>
       </c>
       <c r="K17" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="L17">
         <v>14</v>
@@ -4216,28 +4266,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="T17" t="s">
         <v>131</v>
       </c>
       <c r="U17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="V17" t="s">
         <v>131</v>
       </c>
       <c r="W17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="X17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="CS17">
         <v>34</v>
@@ -4285,7 +4335,7 @@
         <v>141</v>
       </c>
       <c r="DX17" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY17" t="s">
         <v>135</v>
@@ -4293,34 +4343,34 @@
     </row>
     <row r="18" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B18" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F18" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G18" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I18" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J18">
         <v>36</v>
       </c>
       <c r="K18" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L18">
         <v>13</v>
@@ -4329,32 +4379,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S18" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="T18" t="s">
         <v>131</v>
       </c>
       <c r="U18" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="V18" t="s">
         <v>131</v>
       </c>
       <c r="W18" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="X18" t="s">
         <v>131</v>
       </c>
       <c r="Y18" t="s">
-        <v>237</v>
-      </c>
-      <c r="AH18">
-        <f>AI12-AH12</f>
-        <v>-10.689999999999998</v>
+        <v>230</v>
       </c>
       <c r="CS18">
         <v>15</v>
@@ -4399,10 +4445,10 @@
         <v>36</v>
       </c>
       <c r="DW18" t="s">
+        <v>215</v>
+      </c>
+      <c r="DX18" t="s">
         <v>222</v>
-      </c>
-      <c r="DX18" t="s">
-        <v>229</v>
       </c>
       <c r="DY18" t="s">
         <v>135</v>
@@ -4410,19 +4456,19 @@
     </row>
     <row r="19" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F19" t="s">
         <v>131</v>
@@ -4431,16 +4477,16 @@
         <v>130</v>
       </c>
       <c r="H19" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I19" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="J19">
         <v>68</v>
       </c>
       <c r="K19" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="L19">
         <v>15</v>
@@ -4449,25 +4495,22 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="T19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U19" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V19" t="s">
         <v>131</v>
       </c>
       <c r="W19" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="X19" t="s">
         <v>131</v>
       </c>
       <c r="Y19" t="s">
-        <v>242</v>
-      </c>
-      <c r="AH19">
-        <v>-17.3</v>
+        <v>235</v>
       </c>
       <c r="CS19">
         <v>2</v>
@@ -4494,10 +4537,10 @@
         <v>59</v>
       </c>
       <c r="DW19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX19" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY19" t="s">
         <v>135</v>
@@ -4505,37 +4548,37 @@
     </row>
     <row r="20" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E20" t="s">
         <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G20" t="s">
         <v>130</v>
       </c>
       <c r="H20" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I20" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="J20">
         <v>68</v>
       </c>
       <c r="K20" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="L20">
         <v>15</v>
@@ -4547,25 +4590,25 @@
         <v>131</v>
       </c>
       <c r="S20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="T20" t="s">
         <v>131</v>
       </c>
       <c r="U20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V20" t="s">
         <v>131</v>
       </c>
       <c r="W20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="X20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="CS20">
         <v>32</v>
@@ -4601,7 +4644,7 @@
         <v>141</v>
       </c>
       <c r="DX20" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY20" t="s">
         <v>135</v>
@@ -4609,34 +4652,34 @@
     </row>
     <row r="21" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B21" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E21" t="s">
         <v>129</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I21" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J21">
         <v>12</v>
       </c>
       <c r="K21" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -4702,7 +4745,7 @@
         <v>141</v>
       </c>
       <c r="DX21" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY21" t="s">
         <v>135</v>
@@ -4710,34 +4753,34 @@
     </row>
     <row r="22" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E22" t="s">
         <v>129</v>
       </c>
       <c r="F22" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G22" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J22">
         <v>12</v>
       </c>
       <c r="K22" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -4803,7 +4846,7 @@
         <v>141</v>
       </c>
       <c r="DX22" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY22" t="s">
         <v>135</v>
@@ -4811,34 +4854,34 @@
     </row>
     <row r="23" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F23" t="s">
         <v>131</v>
       </c>
       <c r="G23" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J23">
         <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -4850,25 +4893,25 @@
         <v>131</v>
       </c>
       <c r="S23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="T23" t="s">
         <v>131</v>
       </c>
       <c r="U23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="V23" t="s">
         <v>131</v>
       </c>
       <c r="W23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="X23" t="s">
         <v>131</v>
       </c>
       <c r="Y23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="CS23">
         <v>1</v>
@@ -4901,10 +4944,10 @@
         <v>24</v>
       </c>
       <c r="DW23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX23" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY23" t="s">
         <v>135</v>
@@ -4912,34 +4955,34 @@
     </row>
     <row r="24" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E24" t="s">
         <v>129</v>
       </c>
       <c r="F24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G24" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J24">
         <v>16</v>
       </c>
       <c r="K24" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L24">
         <v>12</v>
@@ -4951,13 +4994,13 @@
         <v>131</v>
       </c>
       <c r="W24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X24" t="s">
         <v>131</v>
       </c>
       <c r="Y24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CS24">
         <v>6</v>
@@ -4969,7 +5012,7 @@
         <v>141</v>
       </c>
       <c r="DX24" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY24" t="s">
         <v>135</v>
@@ -4977,16 +5020,16 @@
     </row>
     <row r="25" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B25" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E25" t="s">
         <v>129</v>
@@ -4995,16 +5038,16 @@
         <v>144</v>
       </c>
       <c r="G25" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J25">
         <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L25">
         <v>12</v>
@@ -5016,13 +5059,13 @@
         <v>131</v>
       </c>
       <c r="W25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X25" t="s">
         <v>131</v>
       </c>
       <c r="Y25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CS25">
         <v>1</v>
@@ -5034,7 +5077,7 @@
         <v>141</v>
       </c>
       <c r="DX25" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY25" t="s">
         <v>135</v>
@@ -5042,34 +5085,34 @@
     </row>
     <row r="26" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F26" t="s">
         <v>131</v>
       </c>
       <c r="G26" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J26">
         <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L26">
         <v>12</v>
@@ -5081,13 +5124,13 @@
         <v>131</v>
       </c>
       <c r="W26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X26" t="s">
         <v>131</v>
       </c>
       <c r="Y26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CS26">
         <v>0</v>
@@ -5096,10 +5139,10 @@
         <v>16</v>
       </c>
       <c r="DW26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX26" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY26" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
minor edits and comments
comments on methods checklist document

chunks options added
</commit_message>
<xml_diff>
--- a/data/LSR3_H_2023-11-24.xlsx
+++ b/data/LSR3_H_2023-11-24.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/LRZ Sync+Share/Projects/GALENOS/3. systematic reviews/taar/4_analysis/lsr3_rmarkdown/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/Documents/GitHub/LSR3_taar1_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000ACE7-8810-264A-A282-D65E07339DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F90A78D-2D8B-6E49-9E49-54D20F682AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21880" yWindow="-18280" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="245">
   <si>
     <t>arm_name</t>
   </si>
@@ -472,9 +472,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Isaacson (2023)</t>
   </si>
   <si>
@@ -544,9 +541,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>Koblan (2020)</t>
   </si>
   <si>
@@ -595,18 +589,12 @@
     <t>&gt;18</t>
   </si>
   <si>
-    <t>145</t>
-  </si>
-  <si>
     <t>ulotaront 75mg/d (adults)</t>
   </si>
   <si>
     <t>75</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
     <t>placebo (adults)</t>
   </si>
   <si>
@@ -619,19 +607,10 @@
     <t>464</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
     <t>ulotaront 100mg/d</t>
   </si>
   <si>
     <t>100</t>
-  </si>
-  <si>
-    <t>31</t>
   </si>
   <si>
     <t>24</t>
@@ -811,12 +790,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -831,11 +822,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,14 +1137,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DY26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="34" max="34" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:129" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1546,34 +1542,34 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
         <v>129</v>
       </c>
       <c r="F2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" t="s">
         <v>149</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>150</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>151</v>
-      </c>
-      <c r="I2" t="s">
-        <v>152</v>
       </c>
       <c r="J2">
         <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L2">
         <v>4</v>
@@ -1582,19 +1578,19 @@
         <v>6</v>
       </c>
       <c r="N2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" t="s">
         <v>154</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>155</v>
-      </c>
-      <c r="R2" t="s">
-        <v>156</v>
       </c>
       <c r="S2" t="s">
         <v>144</v>
       </c>
       <c r="T2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U2" t="s">
         <v>144</v>
@@ -1606,31 +1602,31 @@
         <v>144</v>
       </c>
       <c r="X2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y2" t="s">
         <v>144</v>
       </c>
       <c r="Z2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB2" t="s">
         <v>159</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE2" t="s">
         <v>159</v>
       </c>
-      <c r="AB2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>160</v>
-      </c>
       <c r="AF2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG2">
         <v>23</v>
@@ -1651,7 +1647,7 @@
         <v>135</v>
       </c>
       <c r="AN2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AO2">
         <v>24</v>
@@ -1675,7 +1671,7 @@
         <v>135</v>
       </c>
       <c r="BL2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BM2">
         <v>23</v>
@@ -1732,7 +1728,7 @@
         <v>141</v>
       </c>
       <c r="DX2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY2" t="s">
         <v>135</v>
@@ -1740,37 +1736,37 @@
     </row>
     <row r="3" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
         <v>131</v>
       </c>
       <c r="G3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" t="s">
         <v>150</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>151</v>
-      </c>
-      <c r="I3" t="s">
-        <v>152</v>
       </c>
       <c r="J3">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1779,55 +1775,55 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O3" t="s">
         <v>145</v>
       </c>
       <c r="R3" t="s">
+        <v>166</v>
+      </c>
+      <c r="S3" t="s">
         <v>167</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>168</v>
       </c>
-      <c r="T3" t="s">
-        <v>169</v>
-      </c>
       <c r="U3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V3" t="s">
         <v>131</v>
       </c>
       <c r="W3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X3" t="s">
         <v>131</v>
       </c>
       <c r="Y3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB3" t="s">
         <v>159</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE3" t="s">
         <v>159</v>
       </c>
-      <c r="AB3" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>160</v>
-      </c>
       <c r="AF3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG3">
         <v>14</v>
@@ -1848,7 +1844,7 @@
         <v>135</v>
       </c>
       <c r="AN3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AO3">
         <v>14</v>
@@ -1872,7 +1868,7 @@
         <v>135</v>
       </c>
       <c r="BL3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BM3">
         <v>14</v>
@@ -1944,10 +1940,10 @@
         <v>14</v>
       </c>
       <c r="DW3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY3" t="s">
         <v>135</v>
@@ -1958,34 +1954,34 @@
         <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
         <v>129</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G4" t="s">
         <v>130</v>
       </c>
       <c r="H4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J4">
         <v>120</v>
       </c>
       <c r="K4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L4">
         <v>43</v>
@@ -1997,49 +1993,49 @@
         <v>142</v>
       </c>
       <c r="O4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="T4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="V4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="X4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Z4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF4" t="s">
         <v>132</v>
@@ -2162,7 +2158,7 @@
         <v>135</v>
       </c>
       <c r="CJ4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CK4" t="s">
         <v>140</v>
@@ -2255,7 +2251,7 @@
         <v>141</v>
       </c>
       <c r="DX4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY4" t="s">
         <v>135</v>
@@ -2263,19 +2259,19 @@
     </row>
     <row r="5" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" t="s">
         <v>131</v>
@@ -2284,16 +2280,16 @@
         <v>130</v>
       </c>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J5">
         <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L5">
         <v>46</v>
@@ -2302,52 +2298,52 @@
         <v>4</v>
       </c>
       <c r="N5" t="s">
+        <v>176</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="R5" t="s">
+        <v>174</v>
+      </c>
+      <c r="S5" t="s">
+        <v>177</v>
+      </c>
+      <c r="T5" t="s">
         <v>178</v>
       </c>
-      <c r="O5" t="s">
-        <v>179</v>
-      </c>
-      <c r="R5" t="s">
-        <v>176</v>
-      </c>
-      <c r="S5" t="s">
-        <v>179</v>
-      </c>
-      <c r="T5" t="s">
-        <v>180</v>
-      </c>
       <c r="U5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="V5" t="s">
         <v>131</v>
       </c>
       <c r="W5" t="s">
+        <v>177</v>
+      </c>
+      <c r="X5" t="s">
         <v>179</v>
       </c>
-      <c r="X5" t="s">
-        <v>181</v>
-      </c>
       <c r="Y5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Z5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD5" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF5" t="s">
         <v>132</v>
@@ -2470,7 +2466,7 @@
         <v>135</v>
       </c>
       <c r="CJ5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CK5" t="s">
         <v>140</v>
@@ -2560,10 +2556,10 @@
         <v>125</v>
       </c>
       <c r="DW5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY5" t="s">
         <v>135</v>
@@ -2571,76 +2567,85 @@
     </row>
     <row r="6" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
         <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G6" t="s">
         <v>130</v>
       </c>
       <c r="H6" t="s">
-        <v>151</v>
-      </c>
-      <c r="I6" t="s">
-        <v>185</v>
-      </c>
-      <c r="J6">
-        <v>145</v>
+        <v>150</v>
+      </c>
+      <c r="I6" s="2">
+        <v>435</v>
+      </c>
+      <c r="J6" s="3">
+        <v>144</v>
       </c>
       <c r="K6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M6">
         <v>6</v>
       </c>
-      <c r="N6" t="s">
-        <v>146</v>
-      </c>
-      <c r="O6" t="s">
-        <v>187</v>
+      <c r="N6" s="2">
+        <v>22</v>
+      </c>
+      <c r="O6" s="3">
+        <v>144</v>
+      </c>
+      <c r="R6" s="2">
+        <v>34</v>
+      </c>
+      <c r="S6" s="2">
+        <v>144</v>
       </c>
       <c r="Z6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB6" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF6" t="s">
         <v>132</v>
       </c>
-      <c r="AG6">
-        <v>145</v>
+      <c r="AG6" s="2">
+        <v>142</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>102</v>
       </c>
       <c r="AI6">
         <v>-16.899999999999999</v>
       </c>
-      <c r="AJ6">
-        <v>20</v>
+      <c r="AJ6" s="2">
+        <v>19.07</v>
       </c>
       <c r="AK6" t="s">
         <v>133</v>
@@ -2649,13 +2654,13 @@
         <v>134</v>
       </c>
       <c r="AM6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW6" t="s">
         <v>141</v>
       </c>
       <c r="DX6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY6" t="s">
         <v>135</v>
@@ -2663,76 +2668,85 @@
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G7" t="s">
         <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J7">
+        <v>150</v>
+      </c>
+      <c r="I7" s="2">
+        <v>435</v>
+      </c>
+      <c r="J7" s="3">
         <v>145</v>
       </c>
       <c r="K7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
-      <c r="N7" t="s">
-        <v>190</v>
-      </c>
-      <c r="O7" t="s">
-        <v>187</v>
+      <c r="N7" s="2">
+        <v>29</v>
+      </c>
+      <c r="O7" s="3">
+        <v>145</v>
+      </c>
+      <c r="R7" s="2">
+        <v>27</v>
+      </c>
+      <c r="S7" s="2">
+        <v>145</v>
       </c>
       <c r="Z7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA7" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB7" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC7" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF7" t="s">
         <v>132</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="2">
         <v>145</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>102</v>
       </c>
       <c r="AI7">
         <v>-19.600000000000001</v>
       </c>
-      <c r="AJ7">
-        <v>20</v>
+      <c r="AJ7" s="2">
+        <v>19.27</v>
       </c>
       <c r="AK7" t="s">
         <v>133</v>
@@ -2741,13 +2755,13 @@
         <v>134</v>
       </c>
       <c r="AM7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW7" t="s">
         <v>141</v>
       </c>
       <c r="DX7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY7" t="s">
         <v>135</v>
@@ -2755,19 +2769,19 @@
     </row>
     <row r="8" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F8" t="s">
         <v>131</v>
@@ -2776,43 +2790,49 @@
         <v>130</v>
       </c>
       <c r="H8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J8">
-        <v>145</v>
+        <v>183</v>
+      </c>
+      <c r="J8" s="3">
+        <v>146</v>
       </c>
       <c r="K8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M8">
         <v>6</v>
       </c>
-      <c r="N8" t="s">
-        <v>170</v>
-      </c>
-      <c r="O8" t="s">
-        <v>187</v>
+      <c r="N8" s="2">
+        <v>26</v>
+      </c>
+      <c r="O8" s="3">
+        <v>146</v>
+      </c>
+      <c r="R8" s="2">
+        <v>27</v>
+      </c>
+      <c r="S8" s="2">
+        <v>146</v>
       </c>
       <c r="Z8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB8" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF8" t="s">
         <v>132</v>
@@ -2820,11 +2840,14 @@
       <c r="AG8">
         <v>145</v>
       </c>
+      <c r="AH8" s="2">
+        <v>102</v>
+      </c>
       <c r="AI8">
         <v>-19.3</v>
       </c>
-      <c r="AJ8">
-        <v>20</v>
+      <c r="AJ8" s="2">
+        <v>18.059999999999999</v>
       </c>
       <c r="AK8" t="s">
         <v>133</v>
@@ -2833,13 +2856,13 @@
         <v>134</v>
       </c>
       <c r="AM8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY8" t="s">
         <v>135</v>
@@ -2847,76 +2870,85 @@
     </row>
     <row r="9" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
         <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G9" t="s">
         <v>130</v>
       </c>
       <c r="H9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I9" t="s">
-        <v>194</v>
-      </c>
-      <c r="J9">
-        <v>154</v>
+        <v>190</v>
+      </c>
+      <c r="J9" s="2">
+        <v>155</v>
       </c>
       <c r="K9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M9">
         <v>6</v>
       </c>
-      <c r="N9" t="s">
-        <v>195</v>
-      </c>
-      <c r="O9" t="s">
-        <v>196</v>
+      <c r="N9" s="2">
+        <v>23</v>
+      </c>
+      <c r="O9" s="2">
+        <v>155</v>
+      </c>
+      <c r="R9" s="2">
+        <v>34</v>
+      </c>
+      <c r="S9" s="2">
+        <v>155</v>
       </c>
       <c r="Z9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB9" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB9" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF9" t="s">
         <v>132</v>
       </c>
-      <c r="AG9">
-        <v>154</v>
+      <c r="AG9" s="2">
+        <v>153</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>101</v>
       </c>
       <c r="AI9">
         <v>-16.399999999999999</v>
       </c>
-      <c r="AJ9">
-        <v>20</v>
+      <c r="AJ9" s="2">
+        <v>18.55</v>
       </c>
       <c r="AK9" t="s">
         <v>133</v>
@@ -2925,13 +2957,13 @@
         <v>134</v>
       </c>
       <c r="AM9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW9" t="s">
         <v>141</v>
       </c>
       <c r="DX9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY9" t="s">
         <v>135</v>
@@ -2939,76 +2971,85 @@
     </row>
     <row r="10" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
         <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G10" t="s">
         <v>130</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>194</v>
-      </c>
-      <c r="J10">
+        <v>190</v>
+      </c>
+      <c r="J10" s="2">
         <v>154</v>
       </c>
       <c r="K10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M10">
         <v>6</v>
       </c>
-      <c r="N10" t="s">
-        <v>199</v>
-      </c>
-      <c r="O10" t="s">
-        <v>196</v>
+      <c r="N10" s="2">
+        <v>27</v>
+      </c>
+      <c r="O10" s="2">
+        <v>154</v>
+      </c>
+      <c r="R10" s="2">
+        <v>38</v>
+      </c>
+      <c r="S10" s="2">
+        <v>154</v>
       </c>
       <c r="Z10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA10" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB10" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB10" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC10" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF10" t="s">
         <v>132</v>
       </c>
-      <c r="AG10">
-        <v>154</v>
+      <c r="AG10" s="2">
+        <v>152</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>100</v>
       </c>
       <c r="AI10">
         <v>-18.100000000000001</v>
       </c>
-      <c r="AJ10">
-        <v>20</v>
+      <c r="AJ10" s="2">
+        <v>18.489999999999998</v>
       </c>
       <c r="AK10" t="s">
         <v>133</v>
@@ -3017,13 +3058,13 @@
         <v>134</v>
       </c>
       <c r="AM10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW10" t="s">
         <v>141</v>
       </c>
       <c r="DX10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY10" t="s">
         <v>135</v>
@@ -3031,19 +3072,19 @@
     </row>
     <row r="11" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" t="s">
         <v>131</v>
@@ -3052,55 +3093,64 @@
         <v>130</v>
       </c>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I11" t="s">
-        <v>194</v>
-      </c>
-      <c r="J11">
-        <v>154</v>
+        <v>190</v>
+      </c>
+      <c r="J11" s="2">
+        <v>155</v>
       </c>
       <c r="K11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M11">
         <v>6</v>
       </c>
-      <c r="N11" t="s">
-        <v>200</v>
-      </c>
-      <c r="O11" t="s">
-        <v>196</v>
+      <c r="N11" s="2">
+        <v>21</v>
+      </c>
+      <c r="O11" s="2">
+        <v>155</v>
+      </c>
+      <c r="R11" s="2">
+        <v>27</v>
+      </c>
+      <c r="S11" s="2">
+        <v>155</v>
       </c>
       <c r="Z11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA11" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB11" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB11" s="2" t="s">
         <v>160</v>
       </c>
       <c r="AC11" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF11" t="s">
         <v>132</v>
       </c>
-      <c r="AG11">
-        <v>154</v>
+      <c r="AG11" s="2">
+        <v>155</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>100</v>
       </c>
       <c r="AI11">
         <v>-14.3</v>
       </c>
-      <c r="AJ11">
-        <v>20</v>
+      <c r="AJ11" s="2">
+        <v>18.670000000000002</v>
       </c>
       <c r="AK11" t="s">
         <v>133</v>
@@ -3109,13 +3159,13 @@
         <v>134</v>
       </c>
       <c r="AM11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DW11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY11" t="s">
         <v>135</v>
@@ -3123,19 +3173,19 @@
     </row>
     <row r="12" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" t="s">
         <v>131</v>
@@ -3144,16 +3194,16 @@
         <v>130</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J12">
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L12">
         <v>19</v>
@@ -3162,52 +3212,52 @@
         <v>4</v>
       </c>
       <c r="N12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="R12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="S12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="T12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="V12" t="s">
         <v>131</v>
       </c>
       <c r="W12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="X12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="Z12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD12" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF12" t="s">
         <v>132</v>
@@ -3225,7 +3275,7 @@
         <v>20.18</v>
       </c>
       <c r="AK12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL12" t="s">
         <v>135</v>
@@ -3249,7 +3299,7 @@
         <v>6.64</v>
       </c>
       <c r="AS12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT12" t="s">
         <v>135</v>
@@ -3273,7 +3323,7 @@
         <v>5.81</v>
       </c>
       <c r="BA12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB12" t="s">
         <v>135</v>
@@ -3282,7 +3332,7 @@
         <v>135</v>
       </c>
       <c r="BT12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU12">
         <v>54</v>
@@ -3297,7 +3347,7 @@
         <v>4.03</v>
       </c>
       <c r="BY12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ12" t="s">
         <v>135</v>
@@ -3348,10 +3398,10 @@
         <v>72</v>
       </c>
       <c r="DW12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY12" t="s">
         <v>135</v>
@@ -3359,37 +3409,37 @@
     </row>
     <row r="13" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F13" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="G13" t="s">
         <v>130</v>
       </c>
       <c r="H13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I13" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J13">
         <v>71</v>
       </c>
       <c r="K13" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L13">
         <v>19</v>
@@ -3398,52 +3448,52 @@
         <v>4</v>
       </c>
       <c r="N13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O13" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="R13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S13" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="T13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U13" t="s">
-        <v>214</v>
-      </c>
-      <c r="V13" t="s">
-        <v>158</v>
+        <v>207</v>
+      </c>
+      <c r="V13" s="5">
+        <v>0</v>
       </c>
       <c r="W13" t="s">
-        <v>213</v>
-      </c>
-      <c r="X13" t="s">
-        <v>131</v>
+        <v>206</v>
+      </c>
+      <c r="X13" s="5">
+        <v>2</v>
       </c>
       <c r="Y13" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="Z13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD13" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF13" t="s">
         <v>132</v>
@@ -3461,7 +3511,7 @@
         <v>17.03</v>
       </c>
       <c r="AK13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL13" t="s">
         <v>135</v>
@@ -3485,7 +3535,7 @@
         <v>6.14</v>
       </c>
       <c r="AS13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT13" t="s">
         <v>135</v>
@@ -3509,7 +3559,7 @@
         <v>5.85</v>
       </c>
       <c r="BA13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB13" t="s">
         <v>135</v>
@@ -3518,7 +3568,7 @@
         <v>135</v>
       </c>
       <c r="BT13" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU13">
         <v>49</v>
@@ -3533,7 +3583,7 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="BY13" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ13" t="s">
         <v>135</v>
@@ -3587,7 +3637,7 @@
         <v>141</v>
       </c>
       <c r="DX13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY13" t="s">
         <v>135</v>
@@ -3595,37 +3645,37 @@
     </row>
     <row r="14" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F14" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G14" t="s">
         <v>130</v>
       </c>
       <c r="H14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I14" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J14">
         <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L14">
         <v>15</v>
@@ -3634,52 +3684,52 @@
         <v>4</v>
       </c>
       <c r="N14" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" t="s">
+        <v>210</v>
+      </c>
+      <c r="R14" t="s">
         <v>154</v>
       </c>
-      <c r="O14" t="s">
-        <v>217</v>
-      </c>
-      <c r="R14" t="s">
-        <v>155</v>
-      </c>
       <c r="S14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="T14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="V14" t="s">
         <v>131</v>
       </c>
       <c r="W14" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="X14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y14" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="Z14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD14" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF14" t="s">
         <v>132</v>
@@ -3697,7 +3747,7 @@
         <v>17.670000000000002</v>
       </c>
       <c r="AK14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL14" t="s">
         <v>135</v>
@@ -3721,7 +3771,7 @@
         <v>6.5</v>
       </c>
       <c r="AS14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT14" t="s">
         <v>135</v>
@@ -3745,7 +3795,7 @@
         <v>5.41</v>
       </c>
       <c r="BA14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB14" t="s">
         <v>135</v>
@@ -3754,7 +3804,7 @@
         <v>135</v>
       </c>
       <c r="BT14" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU14">
         <v>51</v>
@@ -3769,7 +3819,7 @@
         <v>4.08</v>
       </c>
       <c r="BY14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ14" t="s">
         <v>135</v>
@@ -3823,7 +3873,7 @@
         <v>141</v>
       </c>
       <c r="DX14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY14" t="s">
         <v>135</v>
@@ -3831,37 +3881,37 @@
     </row>
     <row r="15" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G15" t="s">
         <v>130</v>
       </c>
       <c r="H15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I15" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J15">
         <v>74</v>
       </c>
       <c r="K15" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L15">
         <v>18</v>
@@ -3870,52 +3920,52 @@
         <v>4</v>
       </c>
       <c r="N15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O15" t="s">
+        <v>207</v>
+      </c>
+      <c r="R15" t="s">
+        <v>167</v>
+      </c>
+      <c r="S15" t="s">
         <v>214</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>168</v>
       </c>
-      <c r="S15" t="s">
-        <v>221</v>
-      </c>
-      <c r="T15" t="s">
-        <v>169</v>
-      </c>
       <c r="U15" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="V15" t="s">
         <v>131</v>
       </c>
       <c r="W15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="X15" t="s">
         <v>131</v>
       </c>
       <c r="Y15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="Z15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD15" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AF15" t="s">
         <v>132</v>
@@ -3933,7 +3983,7 @@
         <v>15.78</v>
       </c>
       <c r="AK15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL15" t="s">
         <v>135</v>
@@ -3957,7 +4007,7 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="AS15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AT15" t="s">
         <v>135</v>
@@ -3981,7 +4031,7 @@
         <v>5.13</v>
       </c>
       <c r="BA15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BB15" t="s">
         <v>135</v>
@@ -3990,7 +4040,7 @@
         <v>135</v>
       </c>
       <c r="BT15" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="BU15">
         <v>56</v>
@@ -4005,7 +4055,7 @@
         <v>4.09</v>
       </c>
       <c r="BY15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="BZ15" t="s">
         <v>135</v>
@@ -4056,10 +4106,10 @@
         <v>71</v>
       </c>
       <c r="DW15" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="DX15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DY15" t="s">
         <v>135</v>
@@ -4067,34 +4117,34 @@
     </row>
     <row r="16" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B16" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F16" t="s">
         <v>131</v>
       </c>
       <c r="G16" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I16" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J16">
         <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="L16">
         <v>18</v>
@@ -4103,28 +4153,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="T16" t="s">
         <v>131</v>
       </c>
       <c r="U16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="V16" t="s">
         <v>131</v>
       </c>
       <c r="W16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="X16" t="s">
         <v>131</v>
       </c>
       <c r="Y16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="CS16">
         <v>16</v>
@@ -4169,10 +4219,10 @@
         <v>34</v>
       </c>
       <c r="DW16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX16" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY16" t="s">
         <v>135</v>
@@ -4180,34 +4230,34 @@
     </row>
     <row r="17" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
         <v>129</v>
       </c>
       <c r="F17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G17" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I17" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J17">
         <v>35</v>
       </c>
       <c r="K17" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="L17">
         <v>14</v>
@@ -4216,28 +4266,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="T17" t="s">
         <v>131</v>
       </c>
       <c r="U17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="V17" t="s">
         <v>131</v>
       </c>
       <c r="W17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="X17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y17" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="CS17">
         <v>34</v>
@@ -4285,7 +4335,7 @@
         <v>141</v>
       </c>
       <c r="DX17" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY17" t="s">
         <v>135</v>
@@ -4293,34 +4343,34 @@
     </row>
     <row r="18" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B18" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F18" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G18" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I18" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J18">
         <v>36</v>
       </c>
       <c r="K18" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L18">
         <v>13</v>
@@ -4329,32 +4379,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S18" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="T18" t="s">
         <v>131</v>
       </c>
       <c r="U18" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="V18" t="s">
         <v>131</v>
       </c>
       <c r="W18" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="X18" t="s">
         <v>131</v>
       </c>
       <c r="Y18" t="s">
-        <v>237</v>
-      </c>
-      <c r="AH18">
-        <f>AI12-AH12</f>
-        <v>-10.689999999999998</v>
+        <v>230</v>
       </c>
       <c r="CS18">
         <v>15</v>
@@ -4399,10 +4445,10 @@
         <v>36</v>
       </c>
       <c r="DW18" t="s">
+        <v>215</v>
+      </c>
+      <c r="DX18" t="s">
         <v>222</v>
-      </c>
-      <c r="DX18" t="s">
-        <v>229</v>
       </c>
       <c r="DY18" t="s">
         <v>135</v>
@@ -4410,19 +4456,19 @@
     </row>
     <row r="19" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F19" t="s">
         <v>131</v>
@@ -4431,16 +4477,16 @@
         <v>130</v>
       </c>
       <c r="H19" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I19" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="J19">
         <v>68</v>
       </c>
       <c r="K19" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="L19">
         <v>15</v>
@@ -4449,25 +4495,22 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="T19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U19" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V19" t="s">
         <v>131</v>
       </c>
       <c r="W19" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="X19" t="s">
         <v>131</v>
       </c>
       <c r="Y19" t="s">
-        <v>242</v>
-      </c>
-      <c r="AH19">
-        <v>-17.3</v>
+        <v>235</v>
       </c>
       <c r="CS19">
         <v>2</v>
@@ -4494,10 +4537,10 @@
         <v>59</v>
       </c>
       <c r="DW19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX19" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY19" t="s">
         <v>135</v>
@@ -4505,37 +4548,37 @@
     </row>
     <row r="20" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E20" t="s">
         <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G20" t="s">
         <v>130</v>
       </c>
       <c r="H20" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I20" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="J20">
         <v>68</v>
       </c>
       <c r="K20" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="L20">
         <v>15</v>
@@ -4547,25 +4590,25 @@
         <v>131</v>
       </c>
       <c r="S20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="T20" t="s">
         <v>131</v>
       </c>
       <c r="U20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V20" t="s">
         <v>131</v>
       </c>
       <c r="W20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="X20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="CS20">
         <v>32</v>
@@ -4601,7 +4644,7 @@
         <v>141</v>
       </c>
       <c r="DX20" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY20" t="s">
         <v>135</v>
@@ -4609,34 +4652,34 @@
     </row>
     <row r="21" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B21" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E21" t="s">
         <v>129</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I21" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J21">
         <v>12</v>
       </c>
       <c r="K21" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -4702,7 +4745,7 @@
         <v>141</v>
       </c>
       <c r="DX21" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY21" t="s">
         <v>135</v>
@@ -4710,34 +4753,34 @@
     </row>
     <row r="22" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E22" t="s">
         <v>129</v>
       </c>
       <c r="F22" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G22" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J22">
         <v>12</v>
       </c>
       <c r="K22" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -4803,7 +4846,7 @@
         <v>141</v>
       </c>
       <c r="DX22" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY22" t="s">
         <v>135</v>
@@ -4811,34 +4854,34 @@
     </row>
     <row r="23" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F23" t="s">
         <v>131</v>
       </c>
       <c r="G23" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J23">
         <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -4850,25 +4893,25 @@
         <v>131</v>
       </c>
       <c r="S23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="T23" t="s">
         <v>131</v>
       </c>
       <c r="U23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="V23" t="s">
         <v>131</v>
       </c>
       <c r="W23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="X23" t="s">
         <v>131</v>
       </c>
       <c r="Y23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="CS23">
         <v>1</v>
@@ -4901,10 +4944,10 @@
         <v>24</v>
       </c>
       <c r="DW23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX23" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY23" t="s">
         <v>135</v>
@@ -4912,34 +4955,34 @@
     </row>
     <row r="24" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E24" t="s">
         <v>129</v>
       </c>
       <c r="F24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G24" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J24">
         <v>16</v>
       </c>
       <c r="K24" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L24">
         <v>12</v>
@@ -4951,13 +4994,13 @@
         <v>131</v>
       </c>
       <c r="W24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X24" t="s">
         <v>131</v>
       </c>
       <c r="Y24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CS24">
         <v>6</v>
@@ -4969,7 +5012,7 @@
         <v>141</v>
       </c>
       <c r="DX24" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY24" t="s">
         <v>135</v>
@@ -4977,16 +5020,16 @@
     </row>
     <row r="25" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B25" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E25" t="s">
         <v>129</v>
@@ -4995,16 +5038,16 @@
         <v>144</v>
       </c>
       <c r="G25" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J25">
         <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L25">
         <v>12</v>
@@ -5016,13 +5059,13 @@
         <v>131</v>
       </c>
       <c r="W25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X25" t="s">
         <v>131</v>
       </c>
       <c r="Y25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CS25">
         <v>1</v>
@@ -5034,7 +5077,7 @@
         <v>141</v>
       </c>
       <c r="DX25" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY25" t="s">
         <v>135</v>
@@ -5042,34 +5085,34 @@
     </row>
     <row r="26" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F26" t="s">
         <v>131</v>
       </c>
       <c r="G26" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J26">
         <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L26">
         <v>12</v>
@@ -5081,13 +5124,13 @@
         <v>131</v>
       </c>
       <c r="W26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X26" t="s">
         <v>131</v>
       </c>
       <c r="Y26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CS26">
         <v>0</v>
@@ -5096,10 +5139,10 @@
         <v>16</v>
       </c>
       <c r="DW26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="DX26" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="DY26" t="s">
         <v>135</v>

</xml_diff>